<commit_message>
Ne PAULEEN Programm/ new Python programs/ huge
</commit_message>
<xml_diff>
--- a/Berechnung PAULEEN .xlsx
+++ b/Berechnung PAULEEN .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i40014121\Desktop\Bachelorarbeit_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FA37A9-A119-462B-A832-F22C1CEEB3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBFBC61-A60E-4200-84B5-08CC50D281E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="330" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38190" yWindow="1590" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -93,8 +93,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0000000000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -146,12 +148,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -159,7 +158,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -442,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +460,7 @@
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -469,12 +473,12 @@
       <c r="C1">
         <v>28800</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
       <c r="O1" t="s">
         <v>15</v>
       </c>
@@ -486,10 +490,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
@@ -507,22 +511,22 @@
       <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -537,11 +541,11 @@
       <c r="C3">
         <v>8</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <f>$A$3/C3</f>
         <v>3686400</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <f>D3*POWER(2,28)/$A$3</f>
         <v>33554432</v>
       </c>
@@ -552,7 +556,7 @@
       <c r="G3">
         <v>34</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <f>G3-28</f>
         <v>6</v>
       </c>
@@ -580,44 +584,48 @@
         <f>ROUNDUP(M3*512/G3,0)</f>
         <v>136</v>
       </c>
+      <c r="P3" s="9">
+        <f>1/(2*PI()*D3*$P$1)*10^(12)</f>
+        <v>1.0040358469843607</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <f>C3*2</f>
         <v>16</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <f>$A$3/C4</f>
         <v>1843200</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <f>D4*POWER(2,28)/$A$3</f>
         <v>16777216</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>34</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <f t="shared" ref="H4:H12" si="1">G4-28</f>
         <v>6</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <f t="shared" ref="I4:I12" si="2">$A$3/G4</f>
         <v>867388.23529411759</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <f t="shared" ref="J4:J12" si="3">16*16*G4</f>
         <v>8704</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <f t="shared" ref="K4:K12" si="4">J4/($A$3*1000)</f>
         <v>2.9513888888888889E-7</v>
       </c>
@@ -625,53 +633,57 @@
         <f t="shared" ref="L4:L12" si="5">J4/($A$1/$C$1)</f>
         <v>8.5</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <f t="shared" ref="M4:M12" si="6">ROUNDUP(L4,0)</f>
         <v>9</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <f t="shared" ref="N4:N12" si="7">ROUNDUP(M4*512/G4,0)</f>
         <v>136</v>
       </c>
+      <c r="P4" s="9">
+        <f t="shared" ref="P4:P12" si="8">1/(2*PI()*D4*$P$1)*10^(12)</f>
+        <v>2.0080716939687213</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
-        <f t="shared" ref="C5:C12" si="8">C4*2</f>
+      <c r="C5" s="4">
+        <f t="shared" ref="C5:C12" si="9">C4*2</f>
         <v>32</v>
       </c>
-      <c r="D5" s="6">
-        <f t="shared" ref="D4:D12" si="9">$A$3/C5</f>
+      <c r="D5" s="5">
+        <f t="shared" ref="D5:D12" si="10">$A$3/C5</f>
         <v>921600</v>
       </c>
-      <c r="E5" s="6">
-        <f t="shared" ref="E5:E12" si="10">D5*POWER(2,28)/$A$3</f>
+      <c r="E5" s="5">
+        <f t="shared" ref="E5:E12" si="11">D5*POWER(2,28)/$A$3</f>
         <v>8388608</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <f>F5+F5/16</f>
         <v>34</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <f t="shared" si="2"/>
         <v>867388.23529411759</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <f>16*16*G5</f>
         <v>8704</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <f t="shared" si="4"/>
         <v>2.9513888888888889E-7</v>
       </c>
@@ -679,53 +691,57 @@
         <f t="shared" si="5"/>
         <v>8.5</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <f t="shared" si="7"/>
         <v>136</v>
       </c>
+      <c r="P5" s="9">
+        <f t="shared" si="8"/>
+        <v>4.0161433879374426</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
-        <f t="shared" si="8"/>
+      <c r="C6" s="4">
+        <f t="shared" si="9"/>
         <v>64</v>
       </c>
-      <c r="D6" s="6">
-        <f t="shared" si="9"/>
+      <c r="D6" s="5">
+        <f t="shared" si="10"/>
         <v>460800</v>
       </c>
-      <c r="E6" s="6">
-        <f t="shared" si="10"/>
+      <c r="E6" s="5">
+        <f t="shared" si="11"/>
         <v>4194304</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="G6" s="7">
-        <f t="shared" ref="G6:G8" si="11">F6+F6/16</f>
+      <c r="G6" s="6">
+        <f t="shared" ref="G6:G8" si="12">F6+F6/16</f>
         <v>68</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <f t="shared" si="2"/>
         <v>433694.1176470588</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <f>16*16*G6</f>
         <v>17408</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <f t="shared" si="4"/>
         <v>5.9027777777777778E-7</v>
       </c>
@@ -733,53 +749,57 @@
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <f t="shared" si="6"/>
         <v>17</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
         <f t="shared" si="7"/>
         <v>128</v>
       </c>
+      <c r="P6" s="9">
+        <f t="shared" si="8"/>
+        <v>8.0322867758748853</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
-        <f t="shared" si="8"/>
+      <c r="C7" s="4">
+        <f t="shared" si="9"/>
         <v>128</v>
       </c>
-      <c r="D7" s="6">
-        <f t="shared" si="9"/>
+      <c r="D7" s="5">
+        <f t="shared" si="10"/>
         <v>230400</v>
       </c>
-      <c r="E7" s="6">
-        <f t="shared" si="10"/>
+      <c r="E7" s="5">
+        <f t="shared" si="11"/>
         <v>2097152</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="G7" s="7">
-        <f t="shared" si="11"/>
+      <c r="G7" s="6">
+        <f t="shared" si="12"/>
         <v>136</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <f t="shared" si="2"/>
         <v>216847.0588235294</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <f t="shared" si="3"/>
         <v>34816</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <f t="shared" si="4"/>
         <v>1.1805555555555556E-6</v>
       </c>
@@ -787,53 +807,57 @@
         <f t="shared" si="5"/>
         <v>34</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <f t="shared" si="6"/>
         <v>34</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="4">
         <f t="shared" si="7"/>
         <v>128</v>
       </c>
+      <c r="P7" s="7">
+        <f t="shared" si="8"/>
+        <v>16.064573551749771</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
-        <f t="shared" si="8"/>
+      <c r="C8" s="4">
+        <f t="shared" si="9"/>
         <v>256</v>
       </c>
-      <c r="D8" s="6">
-        <f t="shared" si="9"/>
+      <c r="D8" s="5">
+        <f t="shared" si="10"/>
         <v>115200</v>
       </c>
-      <c r="E8" s="6">
-        <f t="shared" si="10"/>
+      <c r="E8" s="5">
+        <f t="shared" si="11"/>
         <v>1048576</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f t="shared" si="0"/>
         <v>256</v>
       </c>
-      <c r="G8" s="7">
-        <f t="shared" si="11"/>
+      <c r="G8" s="6">
+        <f t="shared" si="12"/>
         <v>272</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <f t="shared" si="1"/>
         <v>244</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <f t="shared" si="2"/>
         <v>108423.5294117647</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <f t="shared" si="3"/>
         <v>69632</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <f t="shared" si="4"/>
         <v>2.3611111111111111E-6</v>
       </c>
@@ -841,53 +865,57 @@
         <f t="shared" si="5"/>
         <v>68</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <f t="shared" si="6"/>
         <v>68</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="4">
         <f t="shared" si="7"/>
         <v>128</v>
       </c>
+      <c r="P8" s="7">
+        <f t="shared" si="8"/>
+        <v>32.129147103499541</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4">
         <v>6</v>
       </c>
-      <c r="C9" s="5">
-        <f t="shared" si="8"/>
+      <c r="C9" s="4">
+        <f t="shared" si="9"/>
         <v>512</v>
       </c>
-      <c r="D9" s="6">
-        <f t="shared" si="9"/>
+      <c r="D9" s="5">
+        <f t="shared" si="10"/>
         <v>57600</v>
       </c>
-      <c r="E9" s="6">
-        <f t="shared" si="10"/>
+      <c r="E9" s="5">
+        <f t="shared" si="11"/>
         <v>524288</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <f t="shared" si="0"/>
         <v>512</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <f>C9/16</f>
         <v>32</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <f t="shared" si="2"/>
         <v>921600</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <f t="shared" si="3"/>
         <v>8192</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="4">
         <f t="shared" si="4"/>
         <v>2.7777777777777776E-7</v>
       </c>
@@ -895,53 +923,57 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="4">
         <f t="shared" si="7"/>
         <v>128</v>
       </c>
+      <c r="P9" s="7">
+        <f t="shared" si="8"/>
+        <v>64.258294206999082</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4">
         <v>7</v>
       </c>
-      <c r="C10" s="5">
-        <f t="shared" si="8"/>
+      <c r="C10" s="4">
+        <f t="shared" si="9"/>
         <v>1024</v>
       </c>
-      <c r="D10" s="6">
-        <f t="shared" si="9"/>
+      <c r="D10" s="5">
+        <f t="shared" si="10"/>
         <v>28800</v>
       </c>
-      <c r="E10" s="6">
-        <f t="shared" si="10"/>
+      <c r="E10" s="5">
+        <f t="shared" si="11"/>
         <v>262144</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>1024</v>
       </c>
-      <c r="G10" s="7">
-        <f t="shared" ref="G10:G11" si="12">C10/16</f>
+      <c r="G10" s="6">
+        <f t="shared" ref="G10:G11" si="13">C10/16</f>
         <v>64</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <f t="shared" si="2"/>
         <v>460800</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <f t="shared" si="3"/>
         <v>16384</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="4">
         <f t="shared" si="4"/>
         <v>5.5555555555555552E-7</v>
       </c>
@@ -949,53 +981,57 @@
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="4">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="4">
         <f t="shared" si="7"/>
         <v>128</v>
       </c>
+      <c r="P10" s="10">
+        <f t="shared" si="8"/>
+        <v>128.51658841399816</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4">
         <v>8</v>
       </c>
-      <c r="C11" s="5">
-        <f t="shared" si="8"/>
+      <c r="C11" s="4">
+        <f t="shared" si="9"/>
         <v>2048</v>
       </c>
-      <c r="D11" s="6">
-        <f t="shared" si="9"/>
+      <c r="D11" s="5">
+        <f t="shared" si="10"/>
         <v>14400</v>
       </c>
-      <c r="E11" s="6">
-        <f t="shared" si="10"/>
+      <c r="E11" s="5">
+        <f t="shared" si="11"/>
         <v>131072</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f t="shared" si="0"/>
         <v>2048</v>
       </c>
-      <c r="G11" s="7">
-        <f t="shared" si="12"/>
+      <c r="G11" s="6">
+        <f t="shared" si="13"/>
         <v>128</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <f t="shared" si="2"/>
         <v>230400</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="4">
         <f t="shared" si="3"/>
         <v>32768</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="4">
         <f t="shared" si="4"/>
         <v>1.111111111111111E-6</v>
       </c>
@@ -1003,13 +1039,17 @@
         <f t="shared" si="5"/>
         <v>32</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="4">
         <f t="shared" si="6"/>
         <v>32</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="4">
         <f t="shared" si="7"/>
         <v>128</v>
+      </c>
+      <c r="P11" s="10">
+        <f t="shared" si="8"/>
+        <v>257.03317682799633</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1017,15 +1057,15 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="D12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7200</v>
       </c>
       <c r="E12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>65536</v>
       </c>
       <c r="F12">
@@ -1036,7 +1076,7 @@
         <f>C12/16</f>
         <v>256</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <f t="shared" si="1"/>
         <v>228</v>
       </c>
@@ -1064,6 +1104,58 @@
         <f t="shared" si="7"/>
         <v>128</v>
       </c>
+      <c r="P12" s="10">
+        <f t="shared" si="8"/>
+        <v>514.06635365599266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>F14</f>
+        <v>3728</v>
+      </c>
+      <c r="D14">
+        <f>$A$3/C14</f>
+        <v>7910.7296137339054</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14" si="14" xml:space="preserve"> ROUND(D14*POWER(2,28)/$A$3, 0)</f>
+        <v>72005</v>
+      </c>
+      <c r="F14">
+        <f>16*G14</f>
+        <v>3728</v>
+      </c>
+      <c r="G14" s="6">
+        <v>233</v>
+      </c>
+      <c r="H14">
+        <f>G14-28</f>
+        <v>205</v>
+      </c>
+      <c r="I14">
+        <f>$A$3/G14</f>
+        <v>126571.67381974249</v>
+      </c>
+      <c r="J14">
+        <f>16*16*G14</f>
+        <v>59648</v>
+      </c>
+      <c r="K14">
+        <f>J14/($A$3*1000)</f>
+        <v>2.0225694444444446E-6</v>
+      </c>
+      <c r="L14">
+        <f>J14/($A$1/$C$1)</f>
+        <v>58.25</v>
+      </c>
+      <c r="P14" s="7">
+        <f>1/(2*PI()*D14*$P$1)*10^(12)</f>
+        <v>467.88070469471211</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15">
@@ -1071,46 +1163,46 @@
       </c>
       <c r="C15">
         <f>F15</f>
-        <v>576</v>
+        <v>512</v>
       </c>
       <c r="D15">
         <f>$A$3/C15</f>
-        <v>51200</v>
+        <v>57600</v>
       </c>
       <c r="E15">
-        <f xml:space="preserve"> ROUNDUP(D15*POWER(2,28)/$A$3, 0)</f>
-        <v>466034</v>
+        <f t="shared" ref="E15" si="15" xml:space="preserve"> ROUND(D15*POWER(2,28)/$A$3, 0)</f>
+        <v>524288</v>
       </c>
       <c r="F15">
         <f>16*G15</f>
-        <v>576</v>
-      </c>
-      <c r="G15">
-        <v>36</v>
+        <v>512</v>
+      </c>
+      <c r="G15" s="6">
+        <v>32</v>
       </c>
       <c r="H15">
-        <f>G15-4</f>
-        <v>32</v>
+        <f>G15-28</f>
+        <v>4</v>
       </c>
       <c r="I15">
         <f>$A$3/G15</f>
-        <v>819200</v>
+        <v>921600</v>
       </c>
       <c r="J15">
         <f>16*16*G15</f>
-        <v>9216</v>
+        <v>8192</v>
       </c>
       <c r="K15">
         <f>J15/($A$3*1000)</f>
-        <v>3.1250000000000003E-7</v>
+        <v>2.7777777777777776E-7</v>
       </c>
       <c r="L15">
         <f>J15/($A$1/$C$1)</f>
-        <v>9</v>
-      </c>
-      <c r="P15" s="8">
-        <f xml:space="preserve"> ROUND(1/(2*PI()*D15*$P$1)*10^(12), 0)</f>
-        <v>72</v>
+        <v>8</v>
+      </c>
+      <c r="P15" s="7">
+        <f>1/(2*PI()*D15*$P$1)*10^(12)</f>
+        <v>64.258294206999082</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1119,398 +1211,398 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:C23" si="13">F16</f>
-        <v>624</v>
+        <f t="shared" ref="C16:C23" si="16">F16</f>
+        <v>560</v>
       </c>
       <c r="D16">
         <f>$A$3/C16</f>
-        <v>47261.538461538461</v>
+        <v>52662.857142857145</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E16:E23" si="14" xml:space="preserve"> ROUNDUP(D16*POWER(2,28)/$A$3, 0)</f>
-        <v>430186</v>
+        <f xml:space="preserve"> ROUND(D16*POWER(2,28)/$A$3, 0)</f>
+        <v>479349</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F23" si="15">16*G16</f>
-        <v>624</v>
+        <f t="shared" ref="F16:F23" si="17">16*G16</f>
+        <v>560</v>
       </c>
       <c r="G16">
         <f>G15 + 3</f>
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:H23" si="16">G16-4</f>
-        <v>35</v>
+        <f t="shared" ref="H16:H23" si="18">G16-28</f>
+        <v>7</v>
       </c>
       <c r="I16">
-        <f t="shared" ref="I16:I23" si="17">$A$3/G16</f>
-        <v>756184.61538461538</v>
+        <f t="shared" ref="I16:I23" si="19">$A$3/G16</f>
+        <v>842605.71428571432</v>
       </c>
       <c r="J16">
-        <f t="shared" ref="J16:J23" si="18">16*16*G16</f>
-        <v>9984</v>
+        <f t="shared" ref="J16:J23" si="20">16*16*G16</f>
+        <v>8960</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K23" si="19">J16/($A$3*1000)</f>
-        <v>3.3854166666666667E-7</v>
+        <f t="shared" ref="K16:K23" si="21">J16/($A$3*1000)</f>
+        <v>3.0381944444444446E-7</v>
       </c>
       <c r="L16">
-        <f t="shared" ref="L16:L23" si="20">J16/($A$1/$C$1)</f>
-        <v>9.75</v>
-      </c>
-      <c r="P16" s="8">
-        <f t="shared" ref="P16:P23" si="21">1/(2*PI()*D16*$P$1)*10^(12)</f>
-        <v>78.31479606478014</v>
+        <f t="shared" ref="L16:L23" si="22">J16/($A$1/$C$1)</f>
+        <v>8.75</v>
+      </c>
+      <c r="P16" s="7">
+        <f>1/(2*PI()*D16*$P$1)*10^(12)</f>
+        <v>70.28250928890526</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17">
-        <f xml:space="preserve"> B16 + 1</f>
+        <f t="shared" ref="B17:B23" si="23" xml:space="preserve"> B16 + 1</f>
         <v>2</v>
       </c>
       <c r="C17">
-        <f t="shared" si="13"/>
-        <v>672</v>
+        <f t="shared" si="16"/>
+        <v>608</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:D23" si="22">$A$3/C17</f>
-        <v>43885.714285714283</v>
+        <f t="shared" ref="D17:D23" si="24">$A$3/C17</f>
+        <v>48505.26315789474</v>
       </c>
       <c r="E17">
-        <f t="shared" si="14"/>
-        <v>399458</v>
+        <f xml:space="preserve"> ROUND(D17*POWER(2,28)/$A$3, 0)</f>
+        <v>441506</v>
       </c>
       <c r="F17">
-        <f t="shared" si="15"/>
-        <v>672</v>
+        <f t="shared" si="17"/>
+        <v>608</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17:G23" si="23">G16 + 3</f>
-        <v>42</v>
+        <f t="shared" ref="G17:G23" si="25">G16 + 3</f>
+        <v>38</v>
       </c>
       <c r="H17">
-        <f t="shared" si="16"/>
-        <v>38</v>
+        <f t="shared" si="18"/>
+        <v>10</v>
       </c>
       <c r="I17">
-        <f t="shared" si="17"/>
-        <v>702171.42857142852</v>
+        <f t="shared" si="19"/>
+        <v>776084.21052631584</v>
       </c>
       <c r="J17">
-        <f t="shared" si="18"/>
-        <v>10752</v>
+        <f t="shared" si="20"/>
+        <v>9728</v>
       </c>
       <c r="K17">
-        <f t="shared" si="19"/>
-        <v>3.6458333333333332E-7</v>
+        <f t="shared" si="21"/>
+        <v>3.2986111111111111E-7</v>
       </c>
       <c r="L17">
-        <f t="shared" si="20"/>
-        <v>10.5</v>
-      </c>
-      <c r="P17" s="8">
-        <f t="shared" si="21"/>
-        <v>84.339011146686317</v>
+        <f t="shared" si="22"/>
+        <v>9.5</v>
+      </c>
+      <c r="P17" s="7">
+        <f t="shared" ref="P17:P23" si="26">1/(2*PI()*D17*$P$1)*10^(12)</f>
+        <v>76.306724370811409</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18">
-        <f xml:space="preserve"> B17 + 1</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="C18">
-        <f t="shared" si="13"/>
-        <v>720</v>
+        <f t="shared" si="16"/>
+        <v>656</v>
       </c>
       <c r="D18">
+        <f t="shared" si="24"/>
+        <v>44956.097560975613</v>
+      </c>
+      <c r="E18">
+        <f xml:space="preserve"> ROUND(D18*POWER(2,28)/$A$3, 0)</f>
+        <v>409200</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="17"/>
+        <v>656</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="25"/>
+        <v>41</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="18"/>
+        <v>13</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="19"/>
+        <v>719297.56097560981</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="20"/>
+        <v>10496</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="21"/>
+        <v>3.5590277777777775E-7</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="22"/>
-        <v>40960</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="14"/>
-        <v>372828</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="15"/>
-        <v>720</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="23"/>
-        <v>45</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="16"/>
-        <v>41</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="17"/>
-        <v>655360</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="18"/>
-        <v>11520</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="19"/>
-        <v>3.9062500000000002E-7</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="20"/>
-        <v>11.25</v>
-      </c>
-      <c r="P18" s="8">
-        <f t="shared" si="21"/>
-        <v>90.363226228592467</v>
+        <v>10.25</v>
+      </c>
+      <c r="P18" s="7">
+        <f t="shared" si="26"/>
+        <v>82.330939452717587</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19">
-        <f xml:space="preserve"> B18 + 1</f>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="C19">
-        <f t="shared" si="13"/>
-        <v>768</v>
+        <f t="shared" si="16"/>
+        <v>704</v>
       </c>
       <c r="D19">
+        <f t="shared" si="24"/>
+        <v>41890.909090909088</v>
+      </c>
+      <c r="E19">
+        <f xml:space="preserve"> ROUND(D19*POWER(2,28)/$A$3, 0)</f>
+        <v>381300</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="17"/>
+        <v>704</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="25"/>
+        <v>44</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="18"/>
+        <v>16</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="19"/>
+        <v>670254.54545454541</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="20"/>
+        <v>11264</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="21"/>
+        <v>3.8194444444444445E-7</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="22"/>
-        <v>38400</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="14"/>
-        <v>349526</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="15"/>
-        <v>768</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="23"/>
-        <v>48</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="16"/>
-        <v>44</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="17"/>
-        <v>614400</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="18"/>
-        <v>12288</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666667E-7</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="20"/>
-        <v>12</v>
-      </c>
-      <c r="P19" s="8">
-        <f t="shared" si="21"/>
-        <v>96.38744131049863</v>
+        <v>11</v>
+      </c>
+      <c r="P19" s="7">
+        <f t="shared" si="26"/>
+        <v>88.355154534623765</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20">
-        <f xml:space="preserve"> B19 + 1</f>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="C20">
-        <f t="shared" si="13"/>
-        <v>816</v>
+        <f t="shared" si="16"/>
+        <v>752</v>
       </c>
       <c r="D20">
+        <f t="shared" si="24"/>
+        <v>39217.021276595748</v>
+      </c>
+      <c r="E20">
+        <f xml:space="preserve"> ROUND(D20*POWER(2,28)/$A$3, 0)</f>
+        <v>356962</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="17"/>
+        <v>752</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="25"/>
+        <v>47</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="18"/>
+        <v>19</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="19"/>
+        <v>627472.34042553196</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="20"/>
+        <v>12032</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="21"/>
+        <v>4.079861111111111E-7</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="22"/>
-        <v>36141.176470588238</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="14"/>
-        <v>328966</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="15"/>
-        <v>816</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="23"/>
-        <v>51</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="16"/>
-        <v>47</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="17"/>
-        <v>578258.82352941181</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="18"/>
-        <v>13056</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="19"/>
-        <v>4.4270833333333331E-7</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="20"/>
-        <v>12.75</v>
-      </c>
-      <c r="P20" s="8">
-        <f t="shared" si="21"/>
-        <v>102.41165639240478</v>
+        <v>11.75</v>
+      </c>
+      <c r="P20" s="7">
+        <f t="shared" si="26"/>
+        <v>94.379369616529914</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21">
-        <f xml:space="preserve"> B20 + 1</f>
+        <f t="shared" si="23"/>
         <v>6</v>
       </c>
       <c r="C21">
-        <f t="shared" si="13"/>
-        <v>864</v>
+        <f t="shared" si="16"/>
+        <v>800</v>
       </c>
       <c r="D21">
+        <f t="shared" si="24"/>
+        <v>36864</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21:E23" si="27" xml:space="preserve"> ROUND(D21*POWER(2,28)/$A$3, 0)</f>
+        <v>335544</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="17"/>
+        <v>800</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="25"/>
+        <v>50</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="18"/>
+        <v>22</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="19"/>
+        <v>589824</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="20"/>
+        <v>12800</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="21"/>
+        <v>4.340277777777778E-7</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="22"/>
-        <v>34133.333333333336</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="14"/>
-        <v>310690</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="15"/>
-        <v>864</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="23"/>
-        <v>54</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="16"/>
-        <v>50</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="17"/>
-        <v>546133.33333333337</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="18"/>
-        <v>13824</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="19"/>
-        <v>4.6875000000000001E-7</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="20"/>
-        <v>13.5</v>
-      </c>
-      <c r="P21" s="8">
-        <f t="shared" si="21"/>
-        <v>108.43587147431096</v>
+        <v>12.5</v>
+      </c>
+      <c r="P21" s="7">
+        <f t="shared" si="26"/>
+        <v>100.40358469843608</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22">
-        <f xml:space="preserve"> B21 + 1</f>
+        <f t="shared" si="23"/>
         <v>7</v>
       </c>
       <c r="C22">
-        <f t="shared" si="13"/>
-        <v>912</v>
+        <f t="shared" si="16"/>
+        <v>848</v>
       </c>
       <c r="D22">
+        <f t="shared" si="24"/>
+        <v>34777.358490566039</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="27"/>
+        <v>316551</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="17"/>
+        <v>848</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="25"/>
+        <v>53</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="18"/>
+        <v>25</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="19"/>
+        <v>556437.73584905663</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="20"/>
+        <v>13568</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="21"/>
+        <v>4.6006944444444445E-7</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="22"/>
-        <v>32336.842105263157</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="14"/>
-        <v>294338</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="15"/>
-        <v>912</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="23"/>
-        <v>57</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="16"/>
-        <v>53</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="17"/>
-        <v>517389.4736842105</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="18"/>
-        <v>14592</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="19"/>
-        <v>4.9479166666666666E-7</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="20"/>
-        <v>14.25</v>
-      </c>
-      <c r="P22" s="8">
-        <f t="shared" si="21"/>
-        <v>114.46008655621714</v>
+        <v>13.25</v>
+      </c>
+      <c r="P22" s="7">
+        <f t="shared" si="26"/>
+        <v>106.42779978034224</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23">
-        <f xml:space="preserve"> B22 + 1</f>
+        <f t="shared" si="23"/>
         <v>8</v>
       </c>
       <c r="C23">
-        <f t="shared" si="13"/>
-        <v>960</v>
+        <f t="shared" si="16"/>
+        <v>896</v>
       </c>
       <c r="D23">
+        <f t="shared" si="24"/>
+        <v>32914.285714285717</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="27"/>
+        <v>299593</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="17"/>
+        <v>896</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="25"/>
+        <v>56</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="18"/>
+        <v>28</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="19"/>
+        <v>526628.57142857148</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="20"/>
+        <v>14336</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="21"/>
+        <v>4.8611111111111109E-7</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="22"/>
-        <v>30720</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="14"/>
-        <v>279621</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="15"/>
-        <v>960</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="23"/>
-        <v>60</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="16"/>
-        <v>56</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="17"/>
-        <v>491520</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="18"/>
-        <v>15360</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="19"/>
-        <v>5.2083333333333336E-7</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="20"/>
-        <v>15</v>
-      </c>
-      <c r="P23" s="8">
-        <f t="shared" si="21"/>
-        <v>120.48430163812331</v>
+        <v>14</v>
+      </c>
+      <c r="P23" s="7">
+        <f t="shared" si="26"/>
+        <v>112.45201486224839</v>
       </c>
     </row>
   </sheetData>

</xml_diff>